<commit_message>
GBDS NOVEMBER FILES 2025 - fliqlo@GBDS
</commit_message>
<xml_diff>
--- a/GBDS NOVEMBER FILES 2025/INVENTORY COUNT SHEET 2025.xlsx
+++ b/GBDS NOVEMBER FILES 2025/INVENTORY COUNT SHEET 2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS 2025\6 GBDS JUNE FILES 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS NOVEMBER FILES 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6520EDBE-FB5D-40C7-8582-25E453C1D5AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D5C621-6E56-4244-86A0-B5A4D448802B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D34C963E-9680-4B45-A4EE-B681FF0CEC08}"/>
   </bookViews>
@@ -2998,7 +2998,7 @@
   </sheetPr>
   <dimension ref="A1:AV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A56" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>